<commit_message>
--- ТЗ 2 ---
</commit_message>
<xml_diff>
--- a/Provodnik/_шаблоны/ВСОП_1.xlsx
+++ b/Provodnik/_шаблоны/ВСОП_1.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="28830" windowHeight="6405"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -14,10 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
-  <si>
-    <t>ФИО</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Номер телефона</t>
   </si>
@@ -28,15 +25,9 @@
     <t>Рег. Отделение</t>
   </si>
   <si>
-    <t>ВУЗ</t>
-  </si>
-  <si>
     <t>Форма обучения</t>
   </si>
   <si>
-    <t>Учебный центр</t>
-  </si>
-  <si>
     <t>Гражд-тво</t>
   </si>
   <si>
@@ -49,14 +40,29 @@
     <t>ФИО одного из родителей (полностью)</t>
   </si>
   <si>
-    <t>Год обучения (год выдачи свидетельства)</t>
+    <t>ВУЗ/ССУЗ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Учебный центр (лето) </t>
+  </si>
+  <si>
+    <t>Год обучения (лето)</t>
+  </si>
+  <si>
+    <t>ФИО (полностью)</t>
+  </si>
+  <si>
+    <t>Введение первого компонента вакцины  против коронавирусной инфекции (дата фактическая)</t>
+  </si>
+  <si>
+    <t>Введение второго компонента вакцины против коронавирусной инфекции (дата фактическая)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -79,6 +85,14 @@
       <family val="1"/>
       <charset val="204"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="204"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -88,7 +102,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -111,11 +125,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -146,6 +173,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -451,9 +481,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="90" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="90" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:F1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -461,55 +493,62 @@
     <col min="2" max="2" width="36.28515625" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.85546875" style="3" customWidth="1"/>
     <col min="4" max="4" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="11.5703125" style="3" customWidth="1"/>
-    <col min="9" max="9" width="10.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.5703125" style="3" customWidth="1"/>
-    <col min="11" max="11" width="20.140625" style="10" customWidth="1"/>
-    <col min="12" max="12" width="29.5703125" style="8" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="3"/>
+    <col min="5" max="6" width="16" style="3" customWidth="1"/>
+    <col min="7" max="7" width="14.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="11.5703125" style="3" customWidth="1"/>
+    <col min="11" max="11" width="10.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.5703125" style="3" customWidth="1"/>
+    <col min="13" max="13" width="20.140625" style="10" customWidth="1"/>
+    <col min="14" max="14" width="29.5703125" style="8" customWidth="1"/>
+    <col min="15" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="129" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="K1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="N1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="K1" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" s="6" t="s">
-        <v>10</v>
-      </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="7"/>
       <c r="B2" s="2"/>
       <c r="C2" s="1"/>
@@ -520,8 +559,10 @@
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
-      <c r="K2" s="9"/>
-      <c r="L2" s="7"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="9"/>
+      <c r="N2" s="7"/>
     </row>
   </sheetData>
   <sortState ref="B2:J36">

</xml_diff>